<commit_message>
WIP geautomatiseerde verwerking leden en transacties
</commit_message>
<xml_diff>
--- a/resources/Administratie_sjabloon.xlsx
+++ b/resources/Administratie_sjabloon.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dickk\IdeaProjects\vocalmotion\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A196D37-0F27-4DEB-A16A-C8AD22179300}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6C198D-B620-4158-B052-CC9A5AA00A05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Leden" sheetId="1" r:id="rId1"/>
     <sheet name="Transacties" sheetId="6" r:id="rId2"/>
     <sheet name="Resultaten" sheetId="2" r:id="rId3"/>
     <sheet name="Balans" sheetId="3" r:id="rId4"/>
-    <sheet name="Rekeningschema" sheetId="4" r:id="rId5"/>
-    <sheet name="Standaardwaarden" sheetId="5" r:id="rId6"/>
+    <sheet name="Debiteuren" sheetId="7" r:id="rId5"/>
+    <sheet name="Rekeningschema" sheetId="4" r:id="rId6"/>
+    <sheet name="Standaardwaarden" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
   <si>
     <t>Naam</t>
   </si>
@@ -101,24 +102,12 @@
     <t>Afschrijvingen</t>
   </si>
   <si>
-    <t>Overlopende posten</t>
-  </si>
-  <si>
     <t>Inventaris</t>
   </si>
   <si>
     <t>Apparatuur</t>
   </si>
   <si>
-    <t>&amp;vorigjaar</t>
-  </si>
-  <si>
-    <t>&amp;rapportagejaar</t>
-  </si>
-  <si>
-    <t>Saldo</t>
-  </si>
-  <si>
     <t>Resultatenrekening</t>
   </si>
   <si>
@@ -155,22 +144,75 @@
     <t>Elia</t>
   </si>
   <si>
-    <t>De Schoor</t>
-  </si>
-  <si>
     <t>Herkenning</t>
   </si>
   <si>
     <t>Blom</t>
+  </si>
+  <si>
+    <t>min bedrag</t>
+  </si>
+  <si>
+    <t>max bedrag</t>
+  </si>
+  <si>
+    <t>Schoor</t>
+  </si>
+  <si>
+    <t>tot maand</t>
+  </si>
+  <si>
+    <t>rekening</t>
+  </si>
+  <si>
+    <t>Factuurdatum</t>
+  </si>
+  <si>
+    <t>Factuurnr</t>
+  </si>
+  <si>
+    <t>Betaaldatum</t>
+  </si>
+  <si>
+    <t>Factuurnr betaald</t>
+  </si>
+  <si>
+    <t>betalingsverkeer</t>
+  </si>
+  <si>
+    <t>Bankkosten</t>
+  </si>
+  <si>
+    <t>Contributies</t>
+  </si>
+  <si>
+    <t>Debiteuren</t>
+  </si>
+  <si>
+    <t>Resultaat</t>
+  </si>
+  <si>
+    <t>Bezittingen</t>
+  </si>
+  <si>
+    <t>eigen rekening</t>
+  </si>
+  <si>
+    <t>Saldo rekening courant</t>
+  </si>
+  <si>
+    <t>Saldo spaarrekening</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="6" formatCode="&quot;€&quot;\ #,##0;[Red]&quot;€&quot;\ \-#,##0"/>
+    <numFmt numFmtId="7" formatCode="&quot;€&quot;\ #,##0.00;&quot;€&quot;\ \-#,##0.00"/>
     <numFmt numFmtId="164" formatCode="&quot;€&quot;\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="d/mm/yy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -201,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -211,6 +253,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -525,24 +578,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H2"/>
+  <dimension ref="A2:I43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="47.85546875" customWidth="1"/>
-    <col min="3" max="3" width="56" customWidth="1"/>
+    <col min="3" max="3" width="43.5703125" customWidth="1"/>
     <col min="4" max="4" width="26.7109375" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -557,14 +615,402 @@
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>5</v>
       </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F3" s="7"/>
+      <c r="H3" s="2">
+        <f>IF(AND(NOT(ISBLANK(A3)), ISBLANK(E3), ISBLANK(G3)),12,IF(NOT(ISBLANK(A3)),(IF(ISBLANK(E3), MONTH(G3), 12-MONTH(G3)))))*Standaardwaarden!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <f ca="1">H3 - SUMIFS(Transacties!$F$3:'Transacties'!$F$534,Transacties!$C$3:'Transacties'!$C$534,500,Transacties!$D$3:'Transacties'!$D$534, A3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F4" s="7"/>
+      <c r="H4" s="2">
+        <f>IF(AND(NOT(ISBLANK(A4)), ISBLANK(E4), ISBLANK(G4)),12,IF(NOT(ISBLANK(A4)),(IF(ISBLANK(E4), MONTH(G4), 12-MONTH(G4)))))*Standaardwaarden!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <f ca="1">H4 - SUMIFS(Transacties!$F$3:'Transacties'!$F$534,Transacties!$C$3:'Transacties'!$C$534,500,Transacties!$D$3:'Transacties'!$D$534, A4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F5" s="7"/>
+      <c r="H5" s="2">
+        <f>IF(AND(NOT(ISBLANK(A5)), ISBLANK(E5), ISBLANK(G5)),12,IF(NOT(ISBLANK(A5)),(IF(ISBLANK(E5), MONTH(G5), 12-MONTH(G5)))))*Standaardwaarden!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <f ca="1">H5 - SUMIFS(Transacties!$F$3:'Transacties'!$F$534,Transacties!$C$3:'Transacties'!$C$534,500,Transacties!$D$3:'Transacties'!$D$534, A5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F6" s="7"/>
+      <c r="H6" s="2">
+        <f>IF(AND(NOT(ISBLANK(A6)), ISBLANK(E6), ISBLANK(G6)),12,IF(NOT(ISBLANK(A6)),(IF(ISBLANK(E6), MONTH(G6), 12-MONTH(G6)))))*Standaardwaarden!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
+        <f ca="1">H6 - SUMIFS(Transacties!$F$3:'Transacties'!$F$534,Transacties!$C$3:'Transacties'!$C$534,500,Transacties!$D$3:'Transacties'!$D$534, A6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F7" s="7"/>
+      <c r="H7" s="2">
+        <f>IF(AND(NOT(ISBLANK(A7)), ISBLANK(E7), ISBLANK(G7)),12,IF(NOT(ISBLANK(A7)),(IF(ISBLANK(E7), MONTH(G7), 12-MONTH(G7)))))*Standaardwaarden!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="2">
+        <f ca="1">H7 - SUMIFS(Transacties!$F$3:'Transacties'!$F$534,Transacties!$C$3:'Transacties'!$C$534,500,Transacties!$D$3:'Transacties'!$D$534, A7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F8" s="7"/>
+      <c r="H8" s="2">
+        <f>IF(AND(NOT(ISBLANK(A8)), ISBLANK(E8), ISBLANK(G8)),12,IF(NOT(ISBLANK(A8)),(IF(ISBLANK(E8), MONTH(G8), 12-MONTH(G8)))))*Standaardwaarden!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
+        <f ca="1">H8 - SUMIFS(Transacties!$F$3:'Transacties'!$F$534,Transacties!$C$3:'Transacties'!$C$534,500,Transacties!$D$3:'Transacties'!$D$534, A8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F9" s="7"/>
+      <c r="H9" s="2">
+        <f>IF(AND(NOT(ISBLANK(A9)), ISBLANK(E9), ISBLANK(G9)),12,IF(NOT(ISBLANK(A9)),(IF(ISBLANK(E9), MONTH(G9), 12-MONTH(G9)))))*Standaardwaarden!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="2">
+        <f ca="1">H9 - SUMIFS(Transacties!$F$3:'Transacties'!$F$534,Transacties!$C$3:'Transacties'!$C$534,500,Transacties!$D$3:'Transacties'!$D$534, A9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F10" s="7"/>
+      <c r="H10" s="2">
+        <f>IF(AND(NOT(ISBLANK(A10)), ISBLANK(E10), ISBLANK(G10)),12,IF(NOT(ISBLANK(A10)),(IF(ISBLANK(E10), MONTH(G10), 12-MONTH(G10)))))*Standaardwaarden!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <f ca="1">H10 - SUMIFS(Transacties!$F$3:'Transacties'!$F$534,Transacties!$C$3:'Transacties'!$C$534,500,Transacties!$D$3:'Transacties'!$D$534, A10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F11" s="7"/>
+      <c r="H11" s="2">
+        <f>IF(AND(NOT(ISBLANK(A11)), ISBLANK(E11), ISBLANK(G11)),12,IF(NOT(ISBLANK(A11)),(IF(ISBLANK(E11), MONTH(G11), 12-MONTH(G11)))))*Standaardwaarden!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="2">
+        <f ca="1">H11 - SUMIFS(Transacties!$F$3:'Transacties'!$F$534,Transacties!$C$3:'Transacties'!$C$534,500,Transacties!$D$3:'Transacties'!$D$534, A11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F12" s="7"/>
+      <c r="H12" s="2">
+        <f>IF(AND(NOT(ISBLANK(A12)), ISBLANK(E12), ISBLANK(G12)),12,IF(NOT(ISBLANK(A12)),(IF(ISBLANK(E12), MONTH(G12), 12-MONTH(G12)))))*Standaardwaarden!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="2">
+        <f ca="1">H12 - SUMIFS(Transacties!$F$3:'Transacties'!$F$534,Transacties!$C$3:'Transacties'!$C$534,500,Transacties!$D$3:'Transacties'!$D$534, A12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F13" s="7"/>
+      <c r="H13" s="2">
+        <f>IF(AND(NOT(ISBLANK(A13)), ISBLANK(E13), ISBLANK(G13)),12,IF(NOT(ISBLANK(A13)),(IF(ISBLANK(E13), MONTH(G13), 12-MONTH(G13)))))*Standaardwaarden!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <f ca="1">H13 - SUMIFS(Transacties!$F$3:'Transacties'!$F$534,Transacties!$C$3:'Transacties'!$C$534,500,Transacties!$D$3:'Transacties'!$D$534, A13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F14" s="7"/>
+      <c r="H14" s="2">
+        <f>IF(AND(NOT(ISBLANK(A14)), ISBLANK(E14), ISBLANK(G14)),12,IF(NOT(ISBLANK(A14)),(IF(ISBLANK(E14), MONTH(G14), 12-MONTH(G14)))))*Standaardwaarden!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="2">
+        <f ca="1">H14 - SUMIFS(Transacties!$F$3:'Transacties'!$F$534,Transacties!$C$3:'Transacties'!$C$534,500,Transacties!$D$3:'Transacties'!$D$534, A14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F15" s="7"/>
+      <c r="H15" s="2">
+        <f>IF(AND(NOT(ISBLANK(A15)), ISBLANK(E15), ISBLANK(G15)),12,IF(NOT(ISBLANK(A15)),(IF(ISBLANK(E15), MONTH(G15), 12-MONTH(G15)))))*Standaardwaarden!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="2">
+        <f ca="1">H15 - SUMIFS(Transacties!$F$3:'Transacties'!$F$534,Transacties!$C$3:'Transacties'!$C$534,500,Transacties!$D$3:'Transacties'!$D$534, A15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F16" s="7"/>
+      <c r="H16" s="2">
+        <f>IF(AND(NOT(ISBLANK(A16)), ISBLANK(E16), ISBLANK(G16)),12,IF(NOT(ISBLANK(A16)),(IF(ISBLANK(E16), MONTH(G16), 12-MONTH(G16)))))*Standaardwaarden!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="2">
+        <f ca="1">H16 - SUMIFS(Transacties!$F$3:'Transacties'!$F$534,Transacties!$C$3:'Transacties'!$C$534,500,Transacties!$D$3:'Transacties'!$D$534, A16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F17" s="7"/>
+      <c r="H17" s="2">
+        <f>IF(AND(NOT(ISBLANK(A17)), ISBLANK(E17), ISBLANK(G17)),12,IF(NOT(ISBLANK(A17)),(IF(ISBLANK(E17), MONTH(G17), 12-MONTH(G17)))))*Standaardwaarden!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="2">
+        <f ca="1">H17 - SUMIFS(Transacties!$F$3:'Transacties'!$F$534,Transacties!$C$3:'Transacties'!$C$534,500,Transacties!$D$3:'Transacties'!$D$534, A17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F18" s="7"/>
+      <c r="H18" s="2">
+        <f>IF(AND(NOT(ISBLANK(A18)), ISBLANK(E18), ISBLANK(G18)),12,IF(NOT(ISBLANK(A18)),(IF(ISBLANK(E18), MONTH(G18), 12-MONTH(G18)))))*Standaardwaarden!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <f ca="1">H18 - SUMIFS(Transacties!$F$3:'Transacties'!$F$534,Transacties!$C$3:'Transacties'!$C$534,500,Transacties!$D$3:'Transacties'!$D$534, A18)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F19" s="7"/>
+      <c r="H19" s="2">
+        <f>IF(AND(NOT(ISBLANK(A19)), ISBLANK(E19), ISBLANK(G19)),12,IF(NOT(ISBLANK(A19)),(IF(ISBLANK(E19), MONTH(G19), 12-MONTH(G19)))))*Standaardwaarden!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="2">
+        <f ca="1">H19 - SUMIFS(Transacties!$F$3:'Transacties'!$F$534,Transacties!$C$3:'Transacties'!$C$534,500,Transacties!$D$3:'Transacties'!$D$534, A19)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F20" s="7"/>
+      <c r="H20" s="2">
+        <f>IF(AND(NOT(ISBLANK(A20)), ISBLANK(E20), ISBLANK(G20)),12,IF(NOT(ISBLANK(A20)),(IF(ISBLANK(E20), MONTH(G20), 12-MONTH(G20)))))*Standaardwaarden!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="2">
+        <f ca="1">H20 - SUMIFS(Transacties!$F$3:'Transacties'!$F$534,Transacties!$C$3:'Transacties'!$C$534,500,Transacties!$D$3:'Transacties'!$D$534, A20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F21" s="7"/>
+      <c r="H21" s="2">
+        <f>IF(AND(NOT(ISBLANK(A21)), ISBLANK(E21), ISBLANK(G21)),12,IF(NOT(ISBLANK(A21)),(IF(ISBLANK(E21), MONTH(G21), 12-MONTH(G21)))))*Standaardwaarden!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="2">
+        <f ca="1">H21 - SUMIFS(Transacties!$F$3:'Transacties'!$F$534,Transacties!$C$3:'Transacties'!$C$534,500,Transacties!$D$3:'Transacties'!$D$534, A21)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F22" s="7"/>
+      <c r="H22" s="2">
+        <f>IF(AND(NOT(ISBLANK(A22)), ISBLANK(E22), ISBLANK(G22)),12,IF(NOT(ISBLANK(A22)),(IF(ISBLANK(E22), MONTH(G22), 12-MONTH(G22)))))*Standaardwaarden!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="2">
+        <f ca="1">H22 - SUMIFS(Transacties!$F$3:'Transacties'!$F$534,Transacties!$C$3:'Transacties'!$C$534,500,Transacties!$D$3:'Transacties'!$D$534, A22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F23" s="7"/>
+      <c r="H23" s="2">
+        <f>IF(AND(NOT(ISBLANK(A23)), ISBLANK(E23), ISBLANK(G23)),12,IF(NOT(ISBLANK(A23)),(IF(ISBLANK(E23), MONTH(G23), 12-MONTH(G23)))))*Standaardwaarden!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="I23" s="2">
+        <f ca="1">H23 - SUMIFS(Transacties!$F$3:'Transacties'!$F$534,Transacties!$C$3:'Transacties'!$C$534,500,Transacties!$D$3:'Transacties'!$D$534, A23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F24" s="7"/>
+      <c r="H24" s="2">
+        <f>IF(AND(NOT(ISBLANK(A24)), ISBLANK(E24), ISBLANK(G24)),12,IF(NOT(ISBLANK(A24)),(IF(ISBLANK(E24), MONTH(G24), 12-MONTH(G24)))))*Standaardwaarden!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="I24" s="2">
+        <f ca="1">H24 - SUMIFS(Transacties!$F$3:'Transacties'!$F$534,Transacties!$C$3:'Transacties'!$C$534,500,Transacties!$D$3:'Transacties'!$D$534, A24)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F25" s="7"/>
+      <c r="H25" s="2">
+        <f>IF(AND(NOT(ISBLANK(A25)), ISBLANK(E25), ISBLANK(G25)),12,IF(NOT(ISBLANK(A25)),(IF(ISBLANK(E25), MONTH(G25), 12-MONTH(G25)))))*Standaardwaarden!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="I25" s="2">
+        <f ca="1">H25 - SUMIFS(Transacties!$F$3:'Transacties'!$F$534,Transacties!$C$3:'Transacties'!$C$534,500,Transacties!$D$3:'Transacties'!$D$534, A25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F26" s="7"/>
+      <c r="H26" s="2">
+        <f>IF(AND(NOT(ISBLANK(A26)), ISBLANK(E26), ISBLANK(G26)),12,IF(NOT(ISBLANK(A26)),(IF(ISBLANK(E26), MONTH(G26), 12-MONTH(G26)))))*Standaardwaarden!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="I26" s="2">
+        <f ca="1">H26 - SUMIFS(Transacties!$F$3:'Transacties'!$F$534,Transacties!$C$3:'Transacties'!$C$534,500,Transacties!$D$3:'Transacties'!$D$534, A26)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F27" s="7"/>
+      <c r="H27" s="2">
+        <f>IF(AND(NOT(ISBLANK(A27)), ISBLANK(E27), ISBLANK(G27)),12,IF(NOT(ISBLANK(A27)),(IF(ISBLANK(E27), MONTH(G27), 12-MONTH(G27)))))*Standaardwaarden!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="I27" s="2">
+        <f ca="1">H27 - SUMIFS(Transacties!$F$3:'Transacties'!$F$534,Transacties!$C$3:'Transacties'!$C$534,500,Transacties!$D$3:'Transacties'!$D$534, A27)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F28" s="7"/>
+      <c r="H28" s="2">
+        <f>IF(AND(NOT(ISBLANK(A28)), ISBLANK(E28), ISBLANK(G28)),12,IF(NOT(ISBLANK(A28)),(IF(ISBLANK(E28), MONTH(G28), 12-MONTH(G28)))))*Standaardwaarden!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="I28" s="2">
+        <f ca="1">H28 - SUMIFS(Transacties!$F$3:'Transacties'!$F$534,Transacties!$C$3:'Transacties'!$C$534,500,Transacties!$D$3:'Transacties'!$D$534, A28)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F29" s="7"/>
+      <c r="H29" s="2">
+        <f>IF(AND(NOT(ISBLANK(A29)), ISBLANK(E29), ISBLANK(G29)),12,IF(NOT(ISBLANK(A29)),(IF(ISBLANK(E29), MONTH(G29), 12-MONTH(G29)))))*Standaardwaarden!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="2">
+        <f ca="1">H29 - SUMIFS(Transacties!$F$3:'Transacties'!$F$534,Transacties!$C$3:'Transacties'!$C$534,500,Transacties!$D$3:'Transacties'!$D$534, A29)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F30" s="7"/>
+      <c r="H30" s="2">
+        <f>IF(AND(NOT(ISBLANK(A30)), ISBLANK(E30), ISBLANK(G30)),12,IF(NOT(ISBLANK(A30)),(IF(ISBLANK(E30), MONTH(G30), 12-MONTH(G30)))))*Standaardwaarden!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="I30" s="2">
+        <f ca="1">H30 - SUMIFS(Transacties!$F$3:'Transacties'!$F$534,Transacties!$C$3:'Transacties'!$C$534,500,Transacties!$D$3:'Transacties'!$D$534, A30)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F31" s="7"/>
+      <c r="H31" s="2">
+        <f>IF(AND(NOT(ISBLANK(A31)), ISBLANK(E31), ISBLANK(G31)),12,IF(NOT(ISBLANK(A31)),(IF(ISBLANK(E31), MONTH(G31), 12-MONTH(G31)))))*Standaardwaarden!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="I31" s="2">
+        <f ca="1">H31 - SUMIFS(Transacties!$F$3:'Transacties'!$F$534,Transacties!$C$3:'Transacties'!$C$534,500,Transacties!$D$3:'Transacties'!$D$534, A31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F32" s="7"/>
+      <c r="H32" s="2">
+        <f>IF(AND(NOT(ISBLANK(A32)), ISBLANK(E32), ISBLANK(G32)),12,IF(NOT(ISBLANK(A32)),(IF(ISBLANK(E32), MONTH(G32), 12-MONTH(G32)))))*Standaardwaarden!$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="I32" s="2">
+        <f ca="1">H32 - SUMIFS(Transacties!$F$3:'Transacties'!$F$534,Transacties!$C$3:'Transacties'!$C$534,500,Transacties!$D$3:'Transacties'!$D$534, A32)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F33" s="7"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+    </row>
+    <row r="34" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F34" s="7"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+    </row>
+    <row r="35" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F35" s="7"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+    </row>
+    <row r="36" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F36" s="7"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+    </row>
+    <row r="37" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F37" s="7"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+    </row>
+    <row r="38" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F38" s="7"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+    </row>
+    <row r="39" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F39" s="7"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+    </row>
+    <row r="40" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F40" s="7"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+    </row>
+    <row r="41" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F41" s="7"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+    </row>
+    <row r="42" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F42" s="7"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+    </row>
+    <row r="43" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F43" s="7"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -574,49 +1020,62 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3848252C-EAC0-4885-B267-47F44353D9FA}">
-  <dimension ref="A2:E2"/>
+  <dimension ref="A2:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="111" customWidth="1"/>
+    <col min="1" max="2" width="15.28515625" style="11" customWidth="1"/>
+    <col min="3" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="7" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="85.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>33</v>
-      </c>
+      <c r="F2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,18 +1087,20 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" t="s">
-        <v>24</v>
+        <v>32</v>
+      </c>
+      <c r="C3" s="6">
+        <f>YEAR(Transacties!A3)-1</f>
+        <v>1899</v>
+      </c>
+      <c r="D3">
+        <f>YEAR(Transacties!A3)</f>
+        <v>1900</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -649,6 +1110,14 @@
       <c r="B4" t="s">
         <v>8</v>
       </c>
+      <c r="C4">
+        <f>SUMIF(Transacties!I3:'Transacties'!I500,Transacties!C3=Resultaten!A4)</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <f>SUMIF(Transacties!$C$3:$C$534,A4,Transacties!$F$3:'Transacties'!$F$534)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -657,6 +1126,10 @@
       <c r="B5" t="s">
         <v>10</v>
       </c>
+      <c r="D5" s="2">
+        <f>SUMIF(Transacties!$C$3:$C$534,A5,Transacties!$F$3:'Transacties'!$F$534)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -665,6 +1138,10 @@
       <c r="B6" t="s">
         <v>12</v>
       </c>
+      <c r="D6" s="2">
+        <f>SUMIF(Transacties!$C$3:$C$534,A6,Transacties!$F$3:'Transacties'!$F$534)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -673,6 +1150,10 @@
       <c r="B7" t="s">
         <v>13</v>
       </c>
+      <c r="D7" s="2">
+        <f>SUMIF(Transacties!$C$3:$C$534,A7,Transacties!$F$3:'Transacties'!$F$534)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -681,6 +1162,10 @@
       <c r="B8" t="s">
         <v>14</v>
       </c>
+      <c r="D8" s="2">
+        <f>SUMIF(Transacties!$C$3:$C$534,A8,Transacties!$F$3:'Transacties'!$F$534)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -689,26 +1174,42 @@
       <c r="B9" t="s">
         <v>15</v>
       </c>
+      <c r="D9" s="2">
+        <f>SUMIF(Transacties!$C$3:$C$534,A9,Transacties!$F$3:'Transacties'!$F$534)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>900</v>
+        <v>801</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>46</v>
+      </c>
+      <c r="D10" s="2">
+        <f>SUMIF(Transacties!$C$3:$C$534,A10,Transacties!$F$3:'Transacties'!$F$534)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>25</v>
+        <v>19</v>
+      </c>
+      <c r="D11" s="2">
+        <f>SUMIF(Transacties!$C$3:$C$534,A11,Transacties!$F$3:'Transacties'!$F$534)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="2">
+        <f>SUM(D4:D11)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -718,58 +1219,153 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C3" s="6">
+        <f>YEAR(Transacties!A3)-1</f>
+        <v>1899</v>
+      </c>
+      <c r="D3">
+        <f>YEAR(Transacties!A3)</f>
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>100</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="F5" t="str">
+        <f>IF((C5+Balans!D14)=D5,"OK","Niet alles gerubriceerd, controleer de transacties")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>101</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>300</v>
+      </c>
+      <c r="B7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>400</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="2">
+        <f ca="1">SUM(Debiteuren!D10:D12)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEFAA573-15D3-4E08-88FD-00CA517FBFB7}">
+  <dimension ref="A2:F20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="49.140625" customWidth="1"/>
+    <col min="3" max="4" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2">
+        <f>SUM($C3:$C9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="2">
+        <f ca="1">SUM(Leden!I3:I32)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A2:G16"/>
+  <dimension ref="A2:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,7 +1373,8 @@
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="26.7109375" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="7" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -787,13 +1384,19 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>34</v>
+      </c>
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -847,7 +1450,7 @@
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -861,7 +1464,7 @@
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F7" s="4">
         <v>30</v>
@@ -891,47 +1494,61 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>900</v>
+        <v>801</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>46</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>100</v>
-      </c>
-      <c r="C14" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
+        <v>200</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>300</v>
       </c>
-      <c r="C16" t="s">
-        <v>22</v>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>400</v>
+      </c>
+      <c r="C18" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -939,29 +1556,42 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{445BAF90-CCD9-4237-86A1-CE7D80E12D3C}">
-  <dimension ref="A2:B2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="2">
-        <v>28.5</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="B2" s="5">
+        <v>27.5</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>